<commit_message>
chore: publish ekg IG 1.0.1
</commit_message>
<xml_diff>
--- a/ig/ekg/StructureDefinition-medcom-ekg-recording-bundle.xlsx
+++ b/ig/ekg/StructureDefinition-medcom-ekg-recording-bundle.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -48,7 +48,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-14T12:00:33+00:00</t>
+    <t>2026-01-15T08:05:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
chore: publish ekg IG 1.0.2
</commit_message>
<xml_diff>
--- a/ig/ekg/StructureDefinition-medcom-ekg-recording-bundle.xlsx
+++ b/ig/ekg/StructureDefinition-medcom-ekg-recording-bundle.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-15T08:35:33+00:00</t>
+    <t>2026-01-28T10:08:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1599,7 +1599,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" hidden="true">
+    <row r="3">
       <c r="A3" t="s" s="2">
         <v>85</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" hidden="true">
+    <row r="7">
       <c r="A7" t="s" s="2">
         <v>115</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" hidden="true">
+    <row r="8">
       <c r="A8" t="s" s="2">
         <v>122</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" hidden="true">
+    <row r="9">
       <c r="A9" t="s" s="2">
         <v>131</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>189</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
         <v>193</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" hidden="true">
+    <row r="49">
       <c r="A49" t="s" s="2">
         <v>267</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" hidden="true">
+    <row r="54">
       <c r="A54" t="s" s="2">
         <v>274</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
         <v>275</v>
       </c>
@@ -10555,12 +10555,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AN81">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Publish ekg IG 1.0.2 (#62)
* chore: publish ekg IG 1.0.2

* Update history.html

---------

Co-authored-by: SGA-MedCom <SGA-MedCom@users.noreply.github.com>
Co-authored-by: SGA-MedCom <sga@medcom.dk>
</commit_message>
<xml_diff>
--- a/ig/ekg/StructureDefinition-medcom-ekg-recording-bundle.xlsx
+++ b/ig/ekg/StructureDefinition-medcom-ekg-recording-bundle.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-15T08:35:33+00:00</t>
+    <t>2026-01-28T10:08:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1599,7 +1599,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" hidden="true">
+    <row r="3">
       <c r="A3" t="s" s="2">
         <v>85</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" hidden="true">
+    <row r="7">
       <c r="A7" t="s" s="2">
         <v>115</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" hidden="true">
+    <row r="8">
       <c r="A8" t="s" s="2">
         <v>122</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" hidden="true">
+    <row r="9">
       <c r="A9" t="s" s="2">
         <v>131</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>189</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
         <v>193</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" hidden="true">
+    <row r="49">
       <c r="A49" t="s" s="2">
         <v>267</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" hidden="true">
+    <row r="54">
       <c r="A54" t="s" s="2">
         <v>274</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
         <v>275</v>
       </c>
@@ -10555,12 +10555,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AN81">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>